<commit_message>
validando entrada y mejorando codigo
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -19,47 +19,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>estados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a </t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>s0</t>
   </si>
   <si>
-    <t xml:space="preserve">s0 </t>
-  </si>
-  <si>
     <t>s1</t>
   </si>
   <si>
-    <t xml:space="preserve">s1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">s2 </t>
-  </si>
-  <si>
     <t>s2</t>
   </si>
   <si>
     <t>s3</t>
   </si>
   <si>
-    <t xml:space="preserve">s3 </t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Estados</t>
+  </si>
+  <si>
+    <t>Aceptador</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,70 +375,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
+      <c r="F5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>